<commit_message>
this is the new recommended dir structure for simulation input files
</commit_message>
<xml_diff>
--- a/tests/models/potable_water_treatment_plant_A/input/model_test_pwtp_400ML.xlsx
+++ b/tests/models/potable_water_treatment_plant_A/input/model_test_pwtp_400ML.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/testcode/tests/models/potable_water_treatment_plant_A/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/sira/tests/models/potable_water_treatment_plant_A/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED1B0D0-C4CA-264B-9981-DD24FC8F7EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCE5842-76B1-E248-9537-B652F1D875B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="-21800" windowWidth="28800" windowHeight="16900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system_meta" sheetId="15" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="257">
   <si>
     <t>component_type</t>
   </si>
@@ -3619,8 +3619,8 @@
   </sheetPr>
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3687,8 +3687,12 @@
       <c r="G2" s="60">
         <v>1</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
+      <c r="H2" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
@@ -3712,8 +3716,12 @@
       <c r="G3" s="60">
         <v>1</v>
       </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="H3" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
@@ -3737,8 +3745,12 @@
       <c r="G4" s="60">
         <v>1</v>
       </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="H4" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
@@ -3762,8 +3774,12 @@
       <c r="G5" s="60">
         <v>1</v>
       </c>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
+      <c r="H5" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
@@ -3787,8 +3803,12 @@
       <c r="G6" s="60">
         <v>1</v>
       </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
+      <c r="H6" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
@@ -3812,8 +3832,12 @@
       <c r="G7" s="60">
         <v>1</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
+      <c r="H7" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
@@ -3837,8 +3861,12 @@
       <c r="G8" s="60">
         <v>1</v>
       </c>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
+      <c r="H8" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
@@ -3862,8 +3890,12 @@
       <c r="G9" s="60">
         <v>1</v>
       </c>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
+      <c r="H9" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57" t="s">
@@ -3887,8 +3919,12 @@
       <c r="G10" s="60">
         <v>1</v>
       </c>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
+      <c r="H10" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="57" t="s">
@@ -3912,8 +3948,12 @@
       <c r="G11" s="60">
         <v>1</v>
       </c>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
+      <c r="H11" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="57" t="s">
@@ -3937,8 +3977,12 @@
       <c r="G12" s="60">
         <v>1</v>
       </c>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
+      <c r="H12" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="57" t="s">
@@ -3962,8 +4006,12 @@
       <c r="G13" s="60">
         <v>1</v>
       </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
+      <c r="H13" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="57" t="s">
@@ -3987,8 +4035,12 @@
       <c r="G14" s="60">
         <v>1</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
+      <c r="H14" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
@@ -4012,8 +4064,12 @@
       <c r="G15" s="60">
         <v>1</v>
       </c>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
+      <c r="H15" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="57" t="s">
@@ -4037,8 +4093,12 @@
       <c r="G16" s="60">
         <v>1</v>
       </c>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
+      <c r="H16" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="57" t="s">
@@ -4062,8 +4122,12 @@
       <c r="G17" s="60">
         <v>1</v>
       </c>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
+      <c r="H17" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="57" t="s">
@@ -4087,8 +4151,12 @@
       <c r="G18" s="60">
         <v>1</v>
       </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
+      <c r="H18" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="57" t="s">
@@ -4112,8 +4180,12 @@
       <c r="G19" s="60">
         <v>1</v>
       </c>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
+      <c r="H19" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="57" t="s">
@@ -4137,8 +4209,12 @@
       <c r="G20" s="60">
         <v>1</v>
       </c>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
+      <c r="H20" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="57" t="s">
@@ -4162,8 +4238,12 @@
       <c r="G21" s="60">
         <v>1</v>
       </c>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
+      <c r="H21" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="57" t="s">
@@ -4187,8 +4267,12 @@
       <c r="G22" s="60">
         <v>1</v>
       </c>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
+      <c r="H22" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="57" t="s">
@@ -4212,8 +4296,12 @@
       <c r="G23" s="60">
         <v>1</v>
       </c>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
+      <c r="H23" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="57" t="s">
@@ -4237,8 +4325,12 @@
       <c r="G24" s="60">
         <v>1</v>
       </c>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
+      <c r="H24" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="57" t="s">
@@ -4262,8 +4354,12 @@
       <c r="G25" s="60">
         <v>1</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
+      <c r="H25" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="62" t="s">
@@ -4287,8 +4383,12 @@
       <c r="G26" s="60">
         <v>1</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
+      <c r="H26" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="57" t="s">
@@ -4312,8 +4412,12 @@
       <c r="G27" s="60">
         <v>1</v>
       </c>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
+      <c r="H27" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="57" t="s">
@@ -4337,8 +4441,12 @@
       <c r="G28" s="60">
         <v>1</v>
       </c>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
+      <c r="H28" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="29" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="57" t="s">
@@ -4362,8 +4470,12 @@
       <c r="G29" s="60">
         <v>1</v>
       </c>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
+      <c r="H29" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="57" t="s">
@@ -4387,8 +4499,12 @@
       <c r="G30" s="60">
         <v>1</v>
       </c>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
+      <c r="H30" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="57" t="s">
@@ -4412,8 +4528,12 @@
       <c r="G31" s="60">
         <v>1</v>
       </c>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
+      <c r="H31" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="57" t="s">
@@ -4437,8 +4557,12 @@
       <c r="G32" s="60">
         <v>1</v>
       </c>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
+      <c r="H32" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="57" t="s">
@@ -4462,8 +4586,12 @@
       <c r="G33" s="60">
         <v>1</v>
       </c>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
+      <c r="H33" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="34" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="57" t="s">
@@ -4487,8 +4615,12 @@
       <c r="G34" s="60">
         <v>1</v>
       </c>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
+      <c r="H34" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="35" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="57" t="s">
@@ -4512,8 +4644,12 @@
       <c r="G35" s="60">
         <v>1</v>
       </c>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
+      <c r="H35" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="36" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="57" t="s">
@@ -4537,8 +4673,12 @@
       <c r="G36" s="60">
         <v>1</v>
       </c>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
+      <c r="H36" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="37" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="57" t="s">
@@ -4562,8 +4702,12 @@
       <c r="G37" s="60">
         <v>1</v>
       </c>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
+      <c r="H37" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="38" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="57" t="s">
@@ -4587,8 +4731,12 @@
       <c r="G38" s="60">
         <v>1</v>
       </c>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
+      <c r="H38" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="39" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="57" t="s">
@@ -4612,8 +4760,12 @@
       <c r="G39" s="60">
         <v>1</v>
       </c>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
+      <c r="H39" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="40" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="57" t="s">
@@ -4637,8 +4789,12 @@
       <c r="G40" s="60">
         <v>1</v>
       </c>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
+      <c r="H40" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="41" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="57" t="s">
@@ -4662,8 +4818,12 @@
       <c r="G41" s="60">
         <v>1</v>
       </c>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
+      <c r="H41" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="42" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="57" t="s">
@@ -4687,8 +4847,12 @@
       <c r="G42" s="60">
         <v>1</v>
       </c>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
+      <c r="H42" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="43" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="57" t="s">
@@ -4712,8 +4876,12 @@
       <c r="G43" s="60">
         <v>1</v>
       </c>
-      <c r="H43" s="60"/>
-      <c r="I43" s="60"/>
+      <c r="H43" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="44" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="57" t="s">
@@ -4737,8 +4905,12 @@
       <c r="G44" s="60">
         <v>1</v>
       </c>
-      <c r="H44" s="60"/>
-      <c r="I44" s="60"/>
+      <c r="H44" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="45" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="57" t="s">
@@ -4762,8 +4934,12 @@
       <c r="G45" s="60">
         <v>1</v>
       </c>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
+      <c r="H45" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="46" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="57" t="s">
@@ -4787,8 +4963,12 @@
       <c r="G46" s="60">
         <v>1</v>
       </c>
-      <c r="H46" s="60"/>
-      <c r="I46" s="60"/>
+      <c r="H46" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="47" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="57" t="s">
@@ -4812,8 +4992,12 @@
       <c r="G47" s="60">
         <v>1</v>
       </c>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
+      <c r="H47" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="48" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="57" t="s">
@@ -4837,8 +5021,12 @@
       <c r="G48" s="60">
         <v>1</v>
       </c>
-      <c r="H48" s="60"/>
-      <c r="I48" s="60"/>
+      <c r="H48" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="49" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="57" t="s">
@@ -4862,8 +5050,12 @@
       <c r="G49" s="60">
         <v>1</v>
       </c>
-      <c r="H49" s="60"/>
-      <c r="I49" s="60"/>
+      <c r="H49" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="50" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="57" t="s">
@@ -4887,8 +5079,12 @@
       <c r="G50" s="60">
         <v>1</v>
       </c>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
+      <c r="H50" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="51" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="57" t="s">
@@ -4912,8 +5108,12 @@
       <c r="G51" s="60">
         <v>1</v>
       </c>
-      <c r="H51" s="60"/>
-      <c r="I51" s="60"/>
+      <c r="H51" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="52" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="57" t="s">
@@ -4937,8 +5137,12 @@
       <c r="G52" s="60">
         <v>1</v>
       </c>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
+      <c r="H52" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="53" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="57" t="s">
@@ -4962,8 +5166,12 @@
       <c r="G53" s="60">
         <v>1</v>
       </c>
-      <c r="H53" s="60"/>
-      <c r="I53" s="60"/>
+      <c r="H53" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="54" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="57" t="s">
@@ -4987,8 +5195,12 @@
       <c r="G54" s="60">
         <v>1</v>
       </c>
-      <c r="H54" s="60"/>
-      <c r="I54" s="60"/>
+      <c r="H54" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I54" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="55" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="57" t="s">
@@ -5012,8 +5224,12 @@
       <c r="G55" s="60">
         <v>1</v>
       </c>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
+      <c r="H55" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I55" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="56" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="57" t="s">
@@ -5037,8 +5253,12 @@
       <c r="G56" s="60">
         <v>1</v>
       </c>
-      <c r="H56" s="60"/>
-      <c r="I56" s="60"/>
+      <c r="H56" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="57" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="57" t="s">
@@ -5062,8 +5282,12 @@
       <c r="G57" s="60">
         <v>1</v>
       </c>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
+      <c r="H57" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="58" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="57" t="s">
@@ -5087,8 +5311,12 @@
       <c r="G58" s="60">
         <v>1</v>
       </c>
-      <c r="H58" s="60"/>
-      <c r="I58" s="60"/>
+      <c r="H58" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I58" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="59" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="57" t="s">
@@ -5112,8 +5340,12 @@
       <c r="G59" s="60">
         <v>1</v>
       </c>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
+      <c r="H59" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I59" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="60" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="57" t="s">
@@ -5137,8 +5369,12 @@
       <c r="G60" s="60">
         <v>1</v>
       </c>
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
+      <c r="H60" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I60" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="61" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="57" t="s">
@@ -5162,8 +5398,12 @@
       <c r="G61" s="60">
         <v>1</v>
       </c>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
+      <c r="H61" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I61" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="62" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="57" t="s">
@@ -5187,8 +5427,12 @@
       <c r="G62" s="60">
         <v>1</v>
       </c>
-      <c r="H62" s="60"/>
-      <c r="I62" s="60"/>
+      <c r="H62" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I62" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="63" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="57" t="s">
@@ -5212,8 +5456,12 @@
       <c r="G63" s="60">
         <v>1</v>
       </c>
-      <c r="H63" s="60"/>
-      <c r="I63" s="60"/>
+      <c r="H63" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I63" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="64" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="57" t="s">
@@ -5237,8 +5485,12 @@
       <c r="G64" s="60">
         <v>1</v>
       </c>
-      <c r="H64" s="60"/>
-      <c r="I64" s="60"/>
+      <c r="H64" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I64" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="65" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="57" t="s">
@@ -5262,8 +5514,12 @@
       <c r="G65" s="60">
         <v>1</v>
       </c>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
+      <c r="H65" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I65" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="66" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="57" t="s">
@@ -5287,8 +5543,12 @@
       <c r="G66" s="60">
         <v>1</v>
       </c>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
+      <c r="H66" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="67" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="57" t="s">
@@ -5312,8 +5572,12 @@
       <c r="G67" s="60">
         <v>1</v>
       </c>
-      <c r="H67" s="60"/>
-      <c r="I67" s="60"/>
+      <c r="H67" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="68" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="57" t="s">
@@ -5337,8 +5601,12 @@
       <c r="G68" s="60">
         <v>1</v>
       </c>
-      <c r="H68" s="60"/>
-      <c r="I68" s="60"/>
+      <c r="H68" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I68" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="69" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="57" t="s">
@@ -5362,8 +5630,12 @@
       <c r="G69" s="60">
         <v>1</v>
       </c>
-      <c r="H69" s="60"/>
-      <c r="I69" s="60"/>
+      <c r="H69" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I69" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="70" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="57" t="s">
@@ -5387,8 +5659,12 @@
       <c r="G70" s="60">
         <v>1</v>
       </c>
-      <c r="H70" s="60"/>
-      <c r="I70" s="60"/>
+      <c r="H70" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="71" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="57" t="s">
@@ -5412,8 +5688,12 @@
       <c r="G71" s="60">
         <v>1</v>
       </c>
-      <c r="H71" s="60"/>
-      <c r="I71" s="60"/>
+      <c r="H71" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I71" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="72" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="57" t="s">
@@ -5437,8 +5717,12 @@
       <c r="G72" s="60">
         <v>1</v>
       </c>
-      <c r="H72" s="60"/>
-      <c r="I72" s="60"/>
+      <c r="H72" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I72" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="73" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="57" t="s">
@@ -5462,8 +5746,12 @@
       <c r="G73" s="60">
         <v>1</v>
       </c>
-      <c r="H73" s="60"/>
-      <c r="I73" s="60"/>
+      <c r="H73" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="74" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="57" t="s">
@@ -5487,8 +5775,12 @@
       <c r="G74" s="60">
         <v>1</v>
       </c>
-      <c r="H74" s="60"/>
-      <c r="I74" s="60"/>
+      <c r="H74" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I74" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="75" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="57" t="s">
@@ -5512,8 +5804,12 @@
       <c r="G75" s="60">
         <v>1</v>
       </c>
-      <c r="H75" s="60"/>
-      <c r="I75" s="60"/>
+      <c r="H75" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I75" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="76" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="57" t="s">
@@ -5537,8 +5833,12 @@
       <c r="G76" s="60">
         <v>1</v>
       </c>
-      <c r="H76" s="60"/>
-      <c r="I76" s="60"/>
+      <c r="H76" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I76" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="77" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="57" t="s">
@@ -5562,8 +5862,12 @@
       <c r="G77" s="60">
         <v>1</v>
       </c>
-      <c r="H77" s="60"/>
-      <c r="I77" s="60"/>
+      <c r="H77" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I77" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="78" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="57" t="s">
@@ -5587,8 +5891,12 @@
       <c r="G78" s="60">
         <v>1</v>
       </c>
-      <c r="H78" s="60"/>
-      <c r="I78" s="60"/>
+      <c r="H78" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I78" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="79" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="57" t="s">
@@ -5612,8 +5920,12 @@
       <c r="G79" s="60">
         <v>1</v>
       </c>
-      <c r="H79" s="60"/>
-      <c r="I79" s="60"/>
+      <c r="H79" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I79" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="80" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="57" t="s">
@@ -5637,8 +5949,12 @@
       <c r="G80" s="60">
         <v>1</v>
       </c>
-      <c r="H80" s="60"/>
-      <c r="I80" s="60"/>
+      <c r="H80" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I80" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="81" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="57" t="s">
@@ -5662,8 +5978,12 @@
       <c r="G81" s="60">
         <v>1</v>
       </c>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
+      <c r="H81" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I81" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="82" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="57" t="s">
@@ -5687,8 +6007,12 @@
       <c r="G82" s="60">
         <v>1</v>
       </c>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
+      <c r="H82" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I82" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="83" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="57" t="s">
@@ -5712,8 +6036,12 @@
       <c r="G83" s="60">
         <v>1</v>
       </c>
-      <c r="H83" s="60"/>
-      <c r="I83" s="60"/>
+      <c r="H83" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I83" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="57" t="s">
@@ -5737,8 +6065,12 @@
       <c r="G84" s="60">
         <v>1</v>
       </c>
-      <c r="H84" s="60"/>
-      <c r="I84" s="60"/>
+      <c r="H84" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I84" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="85" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="57" t="s">
@@ -5762,8 +6094,12 @@
       <c r="G85" s="60">
         <v>1</v>
       </c>
-      <c r="H85" s="60"/>
-      <c r="I85" s="60"/>
+      <c r="H85" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="86" spans="1:9" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="57" t="s">
@@ -5787,8 +6123,12 @@
       <c r="G86" s="60">
         <v>1</v>
       </c>
-      <c r="H86" s="60"/>
-      <c r="I86" s="60"/>
+      <c r="H86" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" s="60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D88" s="66"/>
@@ -7647,7 +7987,7 @@
   </sheetPr>
   <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>